<commit_message>
modified nomad_plugin.yaml for movpe1 IKZ
</commit_message>
<xml_diff>
--- a/IKZ_plugin/tests/data/movpe_IKZ/movpe1_growth_parser/deposition_control/deposition_control.xlsx
+++ b/IKZ_plugin/tests/data/movpe_IKZ/movpe1_growth_parser/deposition_control/deposition_control.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Deposition Control" sheetId="1" state="visible" r:id="rId2"/>
@@ -659,7 +659,7 @@
     <t xml:space="preserve">Thursday</t>
   </si>
   <si>
-    <t xml:space="preserve">ahialamiseria</t>
+    <t xml:space="preserve">22-12-16-MA-04-CaO</t>
   </si>
   <si>
     <t xml:space="preserve">04</t>
@@ -1506,7 +1506,7 @@
   </sheetPr>
   <dimension ref="A1:AML186"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -29710,7 +29710,7 @@
   </sheetPr>
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed matching of deposition control in MOVPE 1
</commit_message>
<xml_diff>
--- a/IKZ_plugin/tests/data/movpe_IKZ/movpe1_growth_parser/deposition_control/deposition_control.xlsx
+++ b/IKZ_plugin/tests/data/movpe_IKZ/movpe1_growth_parser/deposition_control/deposition_control.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Deposition Control" sheetId="1" state="visible" r:id="rId2"/>
@@ -356,10 +356,10 @@
     <t xml:space="preserve"># end Header</t>
   </si>
   <si>
-    <t xml:space="preserve">Datum</t>
+    <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Wochentag</t>
+    <t xml:space="preserve">Weekday</t>
   </si>
   <si>
     <t xml:space="preserve">Constant Parameters ID</t>
@@ -1506,8 +1506,8 @@
   </sheetPr>
   <dimension ref="A1:AML186"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29710,8 +29710,8 @@
   </sheetPr>
   <dimension ref="A1:W156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>